<commit_message>
new methods for inserting and removing columns, rows and data
</commit_message>
<xml_diff>
--- a/spec/data/workbook_listobjects.xlsx
+++ b/spec/data/workbook_listobjects.xlsx
@@ -29,9 +29,6 @@
     <t>Time</t>
   </si>
   <si>
-    <t>Date</t>
-  </si>
-  <si>
     <t>Fred</t>
   </si>
   <si>
@@ -44,7 +41,10 @@
     <t>John</t>
   </si>
   <si>
-    <t>Dä%&amp;e</t>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>Price</t>
   </si>
 </sst>
 </file>
@@ -80,10 +80,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -104,9 +103,9 @@
   <tableColumns count="5">
     <tableColumn id="1" name="Number"/>
     <tableColumn id="2" name="Person"/>
-    <tableColumn id="3" name="Dä%&amp;e"/>
+    <tableColumn id="3" name="Amount"/>
     <tableColumn id="4" name="Time"/>
-    <tableColumn id="5" name="Date"/>
+    <tableColumn id="5" name="Price"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -428,7 +427,9 @@
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="D3:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -440,13 +441,13 @@
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G3" t="s">
         <v>2</v>
       </c>
       <c r="H3" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="4:8" x14ac:dyDescent="0.25">
@@ -454,7 +455,7 @@
         <v>3</v>
       </c>
       <c r="E4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F4">
         <v>50</v>
@@ -462,8 +463,8 @@
       <c r="G4" s="1">
         <v>0.5</v>
       </c>
-      <c r="H4" s="2">
-        <v>37692</v>
+      <c r="H4">
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="4:8" x14ac:dyDescent="0.25">
@@ -471,13 +472,13 @@
         <v>2</v>
       </c>
       <c r="E5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G5" s="1">
         <v>0.54166666666666663</v>
       </c>
-      <c r="H5" s="2">
-        <v>20579</v>
+      <c r="H5">
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="4:8" x14ac:dyDescent="0.25">
@@ -485,7 +486,7 @@
         <v>3</v>
       </c>
       <c r="E7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F7">
         <v>100</v>
@@ -493,8 +494,8 @@
       <c r="G7" s="1">
         <v>0.66666666666666663</v>
       </c>
-      <c r="H7" s="2">
-        <v>11078</v>
+      <c r="H7">
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="4:8" x14ac:dyDescent="0.25">
@@ -502,7 +503,7 @@
         <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F9">
         <v>40</v>
@@ -510,8 +511,8 @@
       <c r="G9" s="1">
         <v>0.5</v>
       </c>
-      <c r="H9" s="2">
-        <v>43863</v>
+      <c r="H9">
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ListObject#advanced_filter with help of limit
</commit_message>
<xml_diff>
--- a/spec/data/workbook_listobjects.xlsx
+++ b/spec/data/workbook_listobjects.xlsx
@@ -13,12 +13,15 @@
     <sheet name="Tabelle2" sheetId="2" r:id="rId4"/>
     <sheet name="Tabelle3" sheetId="3" r:id="rId5"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Tabelle1!$D$3:$H$16</definedName>
+  </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Number</t>
   </si>
@@ -38,13 +41,28 @@
     <t>Werner</t>
   </si>
   <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Martha</t>
+  </si>
+  <si>
+    <t>Napoli</t>
+  </si>
+  <si>
     <t>John</t>
   </si>
   <si>
-    <t>Amount</t>
-  </si>
-  <si>
-    <t>Price</t>
+    <t>Eiffel</t>
+  </si>
+  <si>
+    <t>Berta</t>
+  </si>
+  <si>
+    <t>Paul</t>
   </si>
 </sst>
 </file>
@@ -98,8 +116,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="table3" displayName="table3" ref="D3:H9" totalsRowShown="0">
-  <autoFilter ref="D3:H9"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="table3" displayName="table3" ref="D3:H16" totalsRowShown="0">
   <tableColumns count="5">
     <tableColumn id="1" name="Number"/>
     <tableColumn id="2" name="Person"/>
@@ -425,10 +442,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Tabelle1"/>
-  <dimension ref="D3:H9"/>
+  <dimension ref="D3:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -441,13 +458,13 @@
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G3" t="s">
         <v>2</v>
       </c>
       <c r="H3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="4:8" x14ac:dyDescent="0.25">
@@ -455,7 +472,7 @@
         <v>3</v>
       </c>
       <c r="E4" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F4">
         <v>50</v>
@@ -513,6 +530,82 @@
       </c>
       <c r="H9">
         <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D10">
+        <v>3</v>
+      </c>
+      <c r="E10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10">
+        <v>50</v>
+      </c>
+      <c r="G10" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="H10">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D11">
+        <v>3</v>
+      </c>
+      <c r="E11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G11" s="1">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="H11">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D14">
+        <v>3</v>
+      </c>
+      <c r="E14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D15">
+        <v>3</v>
+      </c>
+      <c r="E15" t="s">
+        <v>13</v>
+      </c>
+      <c r="F15">
+        <v>40</v>
+      </c>
+      <c r="G15" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="H15">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="16" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16">
+        <v>20</v>
+      </c>
+      <c r="G16" s="1">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="H16">
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
key value which constitutes a number is independent on type
</commit_message>
<xml_diff>
--- a/spec/data/workbook_listobjects.xlsx
+++ b/spec/data/workbook_listobjects.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="20115" windowHeight="10305" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="72" windowWidth="20112" windowHeight="10308" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Makro2" sheetId="5" r:id="rId1"/>
@@ -420,7 +420,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -433,7 +433,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -445,10 +445,10 @@
   <dimension ref="D3:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="3" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
@@ -490,6 +490,9 @@
       </c>
       <c r="E5" t="s">
         <v>3</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
       </c>
       <c r="G5" s="1">
         <v>0.54166666666666663</v>
@@ -623,7 +626,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -636,7 +639,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>